<commit_message>
Modif feuille de route
</commit_message>
<xml_diff>
--- a/Feuille de route.xlsx
+++ b/Feuille de route.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Priorité 1</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Menu : finir le menu de configuration des touches</t>
+  </si>
+  <si>
+    <t>Ranger le code (supprimer des classes si pas nécessaires)</t>
   </si>
 </sst>
 </file>
@@ -379,16 +382,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="3" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -400,39 +403,48 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>